<commit_message>
Updated assignment tracking spreadsheet.
</commit_message>
<xml_diff>
--- a/Udacity Assignment tracker.xlsx
+++ b/Udacity Assignment tracker.xlsx
@@ -881,7 +881,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
@@ -951,7 +951,7 @@
       <c r="G4" s="13"/>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:8" ht="1.5" customHeight="1">
+    <row r="5" spans="1:8" ht="17.5" customHeight="1">
       <c r="A5" s="14"/>
       <c r="B5" s="15" t="s">
         <v>9</v>
@@ -969,7 +969,8 @@
         <v>43110</v>
       </c>
       <c r="G5" s="19">
-        <v>43201</v>
+        <f>F5</f>
+        <v>43110</v>
       </c>
       <c r="H5" s="19"/>
     </row>
@@ -991,7 +992,8 @@
         <v>43111</v>
       </c>
       <c r="G6" s="19">
-        <v>43201</v>
+        <f>F6</f>
+        <v>43111</v>
       </c>
       <c r="H6" s="24"/>
     </row>
@@ -1013,7 +1015,8 @@
         <v>43111</v>
       </c>
       <c r="G7" s="19">
-        <v>43201</v>
+        <f>F7</f>
+        <v>43111</v>
       </c>
       <c r="H7" s="24"/>
     </row>
@@ -1035,7 +1038,8 @@
         <v>43111</v>
       </c>
       <c r="G8" s="19">
-        <v>43201</v>
+        <f>F8</f>
+        <v>43111</v>
       </c>
       <c r="H8" s="24"/>
     </row>
@@ -1057,7 +1061,8 @@
         <v>43112</v>
       </c>
       <c r="G9" s="19">
-        <v>43201</v>
+        <f>F9</f>
+        <v>43112</v>
       </c>
       <c r="H9" s="24"/>
     </row>
@@ -1079,7 +1084,8 @@
         <v>43116</v>
       </c>
       <c r="G10" s="19">
-        <v>43201</v>
+        <f>F10</f>
+        <v>43116</v>
       </c>
       <c r="H10" s="24"/>
     </row>
@@ -1102,7 +1108,8 @@
         <v>43117</v>
       </c>
       <c r="G11" s="19">
-        <v>43201</v>
+        <f>F11</f>
+        <v>43117</v>
       </c>
       <c r="H11" s="24"/>
     </row>
@@ -1125,7 +1132,8 @@
         <v>43118</v>
       </c>
       <c r="G12" s="19">
-        <v>43201</v>
+        <f t="shared" ref="G12:G26" si="0">F12</f>
+        <v>43118</v>
       </c>
       <c r="H12" s="24"/>
     </row>
@@ -1148,7 +1156,8 @@
         <v>43118</v>
       </c>
       <c r="G13" s="19">
-        <v>43201</v>
+        <f t="shared" si="0"/>
+        <v>43118</v>
       </c>
       <c r="H13" s="24"/>
     </row>
@@ -1171,7 +1180,8 @@
         <v>43122</v>
       </c>
       <c r="G14" s="19">
-        <v>43201</v>
+        <f>F14+2</f>
+        <v>43124</v>
       </c>
       <c r="H14" s="24"/>
     </row>
@@ -1190,11 +1200,12 @@
         <v>29</v>
       </c>
       <c r="F15" s="24">
-        <f>F14+1</f>
-        <v>43123</v>
+        <f>G14</f>
+        <v>43124</v>
       </c>
       <c r="G15" s="19">
-        <v>43201</v>
+        <f>F15+5</f>
+        <v>43129</v>
       </c>
       <c r="H15" s="24"/>
     </row>
@@ -1213,11 +1224,12 @@
         <v>29</v>
       </c>
       <c r="F16" s="24">
-        <f>F15+2</f>
-        <v>43125</v>
+        <f>G15</f>
+        <v>43129</v>
       </c>
       <c r="G16" s="19">
-        <v>43201</v>
+        <f>F16+3</f>
+        <v>43132</v>
       </c>
       <c r="H16" s="24"/>
     </row>
@@ -1236,11 +1248,12 @@
         <v>29</v>
       </c>
       <c r="F17" s="24">
-        <f>F16+4</f>
-        <v>43129</v>
+        <f>G16</f>
+        <v>43132</v>
       </c>
       <c r="G17" s="19">
-        <v>43201</v>
+        <f>F17+6</f>
+        <v>43138</v>
       </c>
       <c r="H17" s="24"/>
     </row>
@@ -1259,11 +1272,12 @@
         <v>29</v>
       </c>
       <c r="F18" s="24">
-        <f>F17+2</f>
-        <v>43131</v>
-      </c>
-      <c r="G18" s="19">
-        <v>43201</v>
+        <f>G17</f>
+        <v>43138</v>
+      </c>
+      <c r="G18" s="24">
+        <f>F18+6</f>
+        <v>43144</v>
       </c>
       <c r="H18" s="24"/>
     </row>
@@ -1282,11 +1296,12 @@
         <v>29</v>
       </c>
       <c r="F19" s="24">
-        <f>F18+5</f>
-        <v>43136</v>
-      </c>
-      <c r="G19" s="19">
-        <v>43201</v>
+        <f>G18</f>
+        <v>43144</v>
+      </c>
+      <c r="G19" s="24">
+        <f>F19+3</f>
+        <v>43147</v>
       </c>
       <c r="H19" s="24"/>
     </row>
@@ -1305,11 +1320,12 @@
         <v>29</v>
       </c>
       <c r="F20" s="24">
-        <f>F19+2</f>
-        <v>43138</v>
+        <f>G19</f>
+        <v>43147</v>
       </c>
       <c r="G20" s="19">
-        <v>43201</v>
+        <f>F20+5</f>
+        <v>43152</v>
       </c>
       <c r="H20" s="24"/>
     </row>
@@ -1328,11 +1344,12 @@
         <v>26</v>
       </c>
       <c r="F21" s="24">
-        <f>F20+2</f>
-        <v>43140</v>
+        <f>G20</f>
+        <v>43152</v>
       </c>
       <c r="G21" s="19">
-        <v>43201</v>
+        <f>F21+5</f>
+        <v>43157</v>
       </c>
       <c r="H21" s="24"/>
     </row>
@@ -1351,11 +1368,12 @@
         <v>29</v>
       </c>
       <c r="F22" s="24">
-        <f>F20+2</f>
-        <v>43140</v>
-      </c>
-      <c r="G22" s="19">
-        <v>43201</v>
+        <f>G21</f>
+        <v>43157</v>
+      </c>
+      <c r="G22" s="24">
+        <f>G21+3</f>
+        <v>43160</v>
       </c>
       <c r="H22" s="24"/>
     </row>
@@ -1374,11 +1392,12 @@
         <v>29</v>
       </c>
       <c r="F23" s="24">
-        <f>F22+4</f>
-        <v>43144</v>
-      </c>
-      <c r="G23" s="19">
-        <v>43201</v>
+        <f>G22</f>
+        <v>43160</v>
+      </c>
+      <c r="G23" s="24">
+        <f>F23+5</f>
+        <v>43165</v>
       </c>
       <c r="H23" s="20"/>
     </row>
@@ -1397,11 +1416,12 @@
         <v>29</v>
       </c>
       <c r="F24" s="24">
-        <f>F23+2</f>
-        <v>43146</v>
-      </c>
-      <c r="G24" s="19">
-        <v>43201</v>
+        <f>G23</f>
+        <v>43165</v>
+      </c>
+      <c r="G24" s="24">
+        <f>F24+6</f>
+        <v>43171</v>
       </c>
       <c r="H24" s="20"/>
     </row>
@@ -1420,11 +1440,12 @@
         <v>29</v>
       </c>
       <c r="F25" s="24">
-        <f>F24+5</f>
-        <v>43151</v>
-      </c>
-      <c r="G25" s="19">
-        <v>43201</v>
+        <f>G24</f>
+        <v>43171</v>
+      </c>
+      <c r="G25" s="24">
+        <f>F25+3</f>
+        <v>43174</v>
       </c>
       <c r="H25" s="20"/>
     </row>
@@ -1443,11 +1464,12 @@
         <v>26</v>
       </c>
       <c r="F26" s="24">
-        <f>F25+2</f>
-        <v>43153</v>
+        <f>G25</f>
+        <v>43174</v>
       </c>
       <c r="G26" s="19">
-        <v>43201</v>
+        <f t="shared" si="0"/>
+        <v>43174</v>
       </c>
       <c r="H26" s="20"/>
     </row>
@@ -1612,7 +1634,7 @@
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D2:G2"/>
   </mergeCells>
-  <conditionalFormatting sqref="G5:G41 F8">
+  <conditionalFormatting sqref="F8:G8 G5:G41">
     <cfRule type="expression" dxfId="6" priority="1">
       <formula>AND(OR($D5="In progress",$D5="Not started" ),OR($G5=TODAY(), $G5=TODAY()+1))</formula>
     </cfRule>
@@ -1632,12 +1654,12 @@
       <formula>RegExMatch(($D5),"Done")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G9:G11 G14 G17 G19 G22 G24 F5:F41">
+  <conditionalFormatting sqref="F5:F41 G9:G26">
     <cfRule type="timePeriod" dxfId="2" priority="5" timePeriod="today">
       <formula>FLOOR(F5,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G9:G11 G14 G17 G19 G22 G24 F5:F41">
+  <conditionalFormatting sqref="F5:F41 G9:G26">
     <cfRule type="expression" dxfId="1" priority="6">
       <formula>AND($F5&lt;TODAY(), OR($D5="In progress", $D5="Not started"))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated assignment tracking data.
</commit_message>
<xml_diff>
--- a/Udacity Assignment tracker.xlsx
+++ b/Udacity Assignment tracker.xlsx
@@ -158,7 +158,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -221,11 +221,6 @@
       <name val="Open Sans"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF008000"/>
-      <name val="Open Sans"/>
-    </font>
-    <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
@@ -387,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -446,9 +441,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -462,7 +454,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -881,7 +873,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
@@ -907,16 +899,16 @@
     </row>
     <row r="2" spans="1:8" ht="44.25" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="41" t="s">
+      <c r="C2" s="39"/>
+      <c r="D2" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="40"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="39"/>
       <c r="H2" s="5"/>
     </row>
     <row r="3" spans="1:8" ht="29.25" customHeight="1">
@@ -969,7 +961,7 @@
         <v>43110</v>
       </c>
       <c r="G5" s="19">
-        <f>F5</f>
+        <f t="shared" ref="G5:G11" si="0">F5</f>
         <v>43110</v>
       </c>
       <c r="H5" s="19"/>
@@ -982,200 +974,200 @@
       <c r="C6" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="23">
         <v>43111</v>
       </c>
       <c r="G6" s="19">
-        <f>F6</f>
+        <f t="shared" si="0"/>
         <v>43111</v>
       </c>
-      <c r="H6" s="24"/>
+      <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:8" ht="12.5">
       <c r="A7" s="20"/>
       <c r="B7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="23">
         <v>43111</v>
       </c>
       <c r="G7" s="19">
-        <f>F7</f>
+        <f t="shared" si="0"/>
         <v>43111</v>
       </c>
-      <c r="H7" s="24"/>
+      <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:8" ht="12.5">
       <c r="A8" s="20"/>
       <c r="B8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="23">
         <v>43111</v>
       </c>
       <c r="G8" s="19">
-        <f>F8</f>
+        <f t="shared" si="0"/>
         <v>43111</v>
       </c>
-      <c r="H8" s="24"/>
+      <c r="H8" s="23"/>
     </row>
     <row r="9" spans="1:8" ht="12.5">
       <c r="A9" s="20"/>
       <c r="B9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="23" t="s">
+      <c r="E9" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="23">
         <v>43112</v>
       </c>
       <c r="G9" s="19">
-        <f>F9</f>
+        <f t="shared" si="0"/>
         <v>43112</v>
       </c>
-      <c r="H9" s="24"/>
+      <c r="H9" s="23"/>
     </row>
     <row r="10" spans="1:8" ht="12.5">
       <c r="A10" s="20"/>
       <c r="B10" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="23" t="s">
+      <c r="D10" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="23">
         <v>43116</v>
       </c>
       <c r="G10" s="19">
-        <f>F10</f>
+        <f t="shared" si="0"/>
         <v>43116</v>
       </c>
-      <c r="H10" s="24"/>
+      <c r="H10" s="23"/>
     </row>
     <row r="11" spans="1:8" ht="12.5">
       <c r="A11" s="20"/>
       <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="23" t="s">
+      <c r="D11" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="24">
+      <c r="F11" s="23">
         <f>F10+1</f>
         <v>43117</v>
       </c>
       <c r="G11" s="19">
-        <f>F11</f>
+        <f t="shared" si="0"/>
         <v>43117</v>
       </c>
-      <c r="H11" s="24"/>
+      <c r="H11" s="23"/>
     </row>
     <row r="12" spans="1:8" ht="12.5">
       <c r="A12" s="20"/>
       <c r="B12" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="23" t="s">
+      <c r="D12" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="23">
         <f>F11+1</f>
         <v>43118</v>
       </c>
       <c r="G12" s="19">
-        <f t="shared" ref="G12:G26" si="0">F12</f>
+        <f t="shared" ref="G12:G26" si="1">F12</f>
         <v>43118</v>
       </c>
-      <c r="H12" s="24"/>
+      <c r="H12" s="23"/>
     </row>
     <row r="13" spans="1:8" ht="12.5">
       <c r="A13" s="20"/>
       <c r="B13" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="23" t="s">
+      <c r="E13" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="24">
+      <c r="F13" s="23">
         <f>F11+1</f>
         <v>43118</v>
       </c>
       <c r="G13" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43118</v>
       </c>
-      <c r="H13" s="24"/>
+      <c r="H13" s="23"/>
     </row>
     <row r="14" spans="1:8" ht="12.5">
       <c r="A14" s="20"/>
       <c r="B14" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="24">
+      <c r="F14" s="23">
         <f>F13+4</f>
         <v>43122</v>
       </c>
@@ -1183,219 +1175,219 @@
         <f>F14+2</f>
         <v>43124</v>
       </c>
-      <c r="H14" s="24"/>
+      <c r="H14" s="23"/>
     </row>
     <row r="15" spans="1:8" ht="12.5">
       <c r="A15" s="20"/>
       <c r="B15" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="24">
-        <f>G14</f>
+      <c r="F15" s="23">
+        <f t="shared" ref="F15:F26" si="2">G14</f>
         <v>43124</v>
       </c>
       <c r="G15" s="19">
         <f>F15+5</f>
         <v>43129</v>
       </c>
-      <c r="H15" s="24"/>
+      <c r="H15" s="23"/>
     </row>
     <row r="16" spans="1:8" ht="12.5">
       <c r="A16" s="20"/>
       <c r="B16" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="24">
-        <f>G15</f>
+      <c r="F16" s="23">
+        <f t="shared" si="2"/>
         <v>43129</v>
       </c>
       <c r="G16" s="19">
         <f>F16+3</f>
         <v>43132</v>
       </c>
-      <c r="H16" s="24"/>
+      <c r="H16" s="23"/>
     </row>
     <row r="17" spans="1:8" ht="12.5">
       <c r="A17" s="20"/>
       <c r="B17" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="23" t="s">
+      <c r="E17" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="24">
-        <f>G16</f>
+      <c r="F17" s="23">
+        <f t="shared" si="2"/>
         <v>43132</v>
       </c>
       <c r="G17" s="19">
         <f>F17+6</f>
         <v>43138</v>
       </c>
-      <c r="H17" s="24"/>
+      <c r="H17" s="23"/>
     </row>
     <row r="18" spans="1:8" ht="12.5">
       <c r="A18" s="20"/>
       <c r="B18" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="26" t="s">
+      <c r="D18" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="23" t="s">
+      <c r="E18" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="24">
-        <f>G17</f>
+      <c r="F18" s="23">
+        <f t="shared" si="2"/>
         <v>43138</v>
       </c>
-      <c r="G18" s="24">
+      <c r="G18" s="23">
         <f>F18+6</f>
         <v>43144</v>
       </c>
-      <c r="H18" s="24"/>
+      <c r="H18" s="23"/>
     </row>
     <row r="19" spans="1:8" ht="12.5">
       <c r="A19" s="20"/>
       <c r="B19" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="24">
-        <f>G18</f>
+      <c r="F19" s="23">
+        <f t="shared" si="2"/>
         <v>43144</v>
       </c>
-      <c r="G19" s="24">
+      <c r="G19" s="23">
         <f>F19+3</f>
         <v>43147</v>
       </c>
-      <c r="H19" s="24"/>
+      <c r="H19" s="23"/>
     </row>
     <row r="20" spans="1:8" ht="12.5">
       <c r="A20" s="20"/>
       <c r="B20" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="24">
-        <f>G19</f>
+      <c r="F20" s="23">
+        <f t="shared" si="2"/>
         <v>43147</v>
       </c>
       <c r="G20" s="19">
         <f>F20+5</f>
         <v>43152</v>
       </c>
-      <c r="H20" s="24"/>
+      <c r="H20" s="23"/>
     </row>
     <row r="21" spans="1:8" ht="12.5">
       <c r="A21" s="20"/>
       <c r="B21" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E21" s="23" t="s">
+      <c r="E21" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F21" s="24">
-        <f>G20</f>
+      <c r="F21" s="23">
+        <f t="shared" si="2"/>
         <v>43152</v>
       </c>
       <c r="G21" s="19">
         <f>F21+5</f>
         <v>43157</v>
       </c>
-      <c r="H21" s="24"/>
+      <c r="H21" s="23"/>
     </row>
     <row r="22" spans="1:8" ht="12.5">
       <c r="A22" s="20"/>
       <c r="B22" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="23" t="s">
+      <c r="E22" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="24">
-        <f>G21</f>
+      <c r="F22" s="23">
+        <f t="shared" si="2"/>
         <v>43157</v>
       </c>
-      <c r="G22" s="24">
+      <c r="G22" s="23">
         <f>G21+3</f>
         <v>43160</v>
       </c>
-      <c r="H22" s="24"/>
+      <c r="H22" s="23"/>
     </row>
     <row r="23" spans="1:8" ht="12.5">
       <c r="A23" s="20"/>
       <c r="B23" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="26" t="s">
+      <c r="D23" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E23" s="23" t="s">
+      <c r="E23" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="24">
-        <f>G22</f>
+      <c r="F23" s="23">
+        <f t="shared" si="2"/>
         <v>43160</v>
       </c>
-      <c r="G23" s="24">
+      <c r="G23" s="23">
         <f>F23+5</f>
         <v>43165</v>
       </c>
@@ -1406,20 +1398,20 @@
       <c r="B24" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="26" t="s">
+      <c r="D24" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="24">
-        <f>G23</f>
+      <c r="F24" s="23">
+        <f t="shared" si="2"/>
         <v>43165</v>
       </c>
-      <c r="G24" s="24">
+      <c r="G24" s="23">
         <f>F24+6</f>
         <v>43171</v>
       </c>
@@ -1430,20 +1422,20 @@
       <c r="B25" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D25" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="23" t="s">
+      <c r="E25" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="24">
-        <f>G24</f>
+      <c r="F25" s="23">
+        <f t="shared" si="2"/>
         <v>43171</v>
       </c>
-      <c r="G25" s="24">
+      <c r="G25" s="23">
         <f>F25+3</f>
         <v>43174</v>
       </c>
@@ -1454,180 +1446,180 @@
       <c r="B26" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="26" t="s">
+      <c r="D26" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E26" s="23" t="s">
+      <c r="E26" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F26" s="24">
-        <f>G25</f>
+      <c r="F26" s="23">
+        <f t="shared" si="2"/>
         <v>43174</v>
       </c>
       <c r="G26" s="19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43174</v>
       </c>
       <c r="H26" s="20"/>
     </row>
     <row r="27" spans="1:8" ht="25">
       <c r="A27" s="20"/>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="29"/>
-      <c r="E27" s="30"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
       <c r="H27" s="20"/>
     </row>
     <row r="28" spans="1:8" ht="12.5">
       <c r="A28" s="20"/>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="31"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
       <c r="H28" s="20"/>
     </row>
     <row r="29" spans="1:8" ht="12.5">
       <c r="A29" s="20"/>
       <c r="B29" s="20"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
       <c r="H29" s="20"/>
     </row>
     <row r="30" spans="1:8" ht="12.5">
       <c r="A30" s="20"/>
       <c r="B30" s="20"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="30"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
       <c r="H30" s="20"/>
     </row>
     <row r="31" spans="1:8" ht="12.5">
       <c r="A31" s="20"/>
       <c r="B31" s="20"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="30"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
       <c r="H31" s="20"/>
     </row>
     <row r="32" spans="1:8" ht="12.5">
       <c r="A32" s="20"/>
       <c r="B32" s="20"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="30"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
+      <c r="C32" s="30"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
       <c r="H32" s="20"/>
     </row>
     <row r="33" spans="1:8" ht="12.5">
       <c r="A33" s="20"/>
       <c r="B33" s="20"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="24"/>
-      <c r="G33" s="24"/>
+      <c r="C33" s="30"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
       <c r="H33" s="20"/>
     </row>
     <row r="34" spans="1:8" ht="12.5">
       <c r="A34" s="20"/>
       <c r="B34" s="20"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="24"/>
-      <c r="G34" s="24"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
       <c r="H34" s="20"/>
     </row>
     <row r="35" spans="1:8" ht="12.5">
       <c r="A35" s="20"/>
       <c r="B35" s="20"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="29"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="24"/>
-      <c r="G35" s="24"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
       <c r="H35" s="20"/>
     </row>
     <row r="36" spans="1:8" ht="12.5">
       <c r="A36" s="20"/>
       <c r="B36" s="20"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="24"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="23"/>
       <c r="H36" s="20"/>
     </row>
     <row r="37" spans="1:8" ht="12.5">
       <c r="A37" s="20"/>
       <c r="B37" s="20"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="24"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="23"/>
+      <c r="G37" s="23"/>
       <c r="H37" s="20"/>
     </row>
     <row r="38" spans="1:8" ht="12.5">
       <c r="A38" s="20"/>
       <c r="B38" s="20"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="24"/>
-      <c r="G38" s="24"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="23"/>
+      <c r="G38" s="23"/>
       <c r="H38" s="20"/>
     </row>
     <row r="39" spans="1:8" ht="12.5">
       <c r="A39" s="20"/>
       <c r="B39" s="20"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
       <c r="H39" s="20"/>
     </row>
     <row r="40" spans="1:8" ht="12.5">
       <c r="A40" s="20"/>
       <c r="B40" s="20"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="24"/>
-      <c r="G40" s="24"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
       <c r="H40" s="20"/>
     </row>
     <row r="41" spans="1:8" ht="12.5" hidden="1">
-      <c r="A41" s="34"/>
-      <c r="B41" s="34"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="37"/>
-      <c r="F41" s="38"/>
-      <c r="G41" s="38"/>
-      <c r="H41" s="34"/>
+      <c r="A41" s="33"/>
+      <c r="B41" s="33"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="35"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1749,80 +1741,80 @@
     </row>
     <row r="6" spans="1:3" ht="12.5">
       <c r="A6" s="20"/>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="24"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:3" ht="12.5">
       <c r="A7" s="20"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="24"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="23"/>
     </row>
     <row r="8" spans="1:3" ht="12.5">
       <c r="A8" s="20"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="24"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="23"/>
     </row>
     <row r="9" spans="1:3" ht="12.5">
       <c r="A9" s="20"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="24"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="23"/>
     </row>
     <row r="10" spans="1:3" ht="12.5">
       <c r="A10" s="20"/>
       <c r="B10" s="20"/>
-      <c r="C10" s="24"/>
+      <c r="C10" s="23"/>
     </row>
     <row r="11" spans="1:3" ht="12.5">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
-      <c r="C11" s="24"/>
+      <c r="C11" s="23"/>
     </row>
     <row r="12" spans="1:3" ht="12.5">
       <c r="A12" s="20"/>
       <c r="B12" s="20"/>
-      <c r="C12" s="24"/>
+      <c r="C12" s="23"/>
     </row>
     <row r="13" spans="1:3" ht="12.5">
       <c r="A13" s="20"/>
       <c r="B13" s="20"/>
-      <c r="C13" s="24"/>
+      <c r="C13" s="23"/>
     </row>
     <row r="14" spans="1:3" ht="12.5">
       <c r="A14" s="20"/>
       <c r="B14" s="20"/>
-      <c r="C14" s="24"/>
+      <c r="C14" s="23"/>
     </row>
     <row r="15" spans="1:3" ht="12.5">
       <c r="A15" s="20"/>
       <c r="B15" s="20"/>
-      <c r="C15" s="24"/>
+      <c r="C15" s="23"/>
     </row>
     <row r="16" spans="1:3" ht="12.5">
       <c r="A16" s="20"/>
       <c r="B16" s="20"/>
-      <c r="C16" s="24"/>
+      <c r="C16" s="23"/>
     </row>
     <row r="17" spans="1:3" ht="12.5">
       <c r="A17" s="20"/>
       <c r="B17" s="20"/>
-      <c r="C17" s="24"/>
+      <c r="C17" s="23"/>
     </row>
     <row r="18" spans="1:3" ht="12.5">
       <c r="A18" s="20"/>
       <c r="B18" s="20"/>
-      <c r="C18" s="24"/>
+      <c r="C18" s="23"/>
     </row>
     <row r="19" spans="1:3" ht="12.5">
       <c r="A19" s="20"/>
       <c r="B19" s="20"/>
-      <c r="C19" s="24"/>
+      <c r="C19" s="23"/>
     </row>
     <row r="20" spans="1:3" ht="12.5">
       <c r="A20" s="20"/>
       <c r="B20" s="20"/>
-      <c r="C20" s="24"/>
+      <c r="C20" s="23"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A5:C20">

</xml_diff>